<commit_message>
added cmd progress output for process_mutants
</commit_message>
<xml_diff>
--- a/PracticeSheet.xlsx
+++ b/PracticeSheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhkh\Documents\UBC\COOP\S2019 CARDONA LAB\High Density Transposon Mutant Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3430BC-C93C-43DF-AB6E-8C771C17245D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF1A8F-E658-40EF-B932-5BDD2EA1270B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="275" yWindow="157" windowWidth="18851" windowHeight="10303" xr2:uid="{F2D4EA85-3696-4C72-B544-258F025EF0EE}"/>
+    <workbookView xWindow="1296" yWindow="1126" windowWidth="18851" windowHeight="10302" xr2:uid="{F2D4EA85-3696-4C72-B544-258F025EF0EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,9 +67,6 @@
     <t>COG</t>
   </si>
   <si>
-    <t>Locus tag</t>
-  </si>
-  <si>
     <t>at</t>
   </si>
   <si>
@@ -145,6 +143,9 @@
   </si>
   <si>
     <t>mbc</t>
+  </si>
+  <si>
+    <t>Locus TAG</t>
   </si>
 </sst>
 </file>
@@ -496,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD4661C-C763-4B6E-9515-401C70A35075}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18:N18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -527,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -556,10 +557,10 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2">
         <v>9</v>
@@ -588,10 +589,10 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3">
         <v>10</v>
@@ -620,10 +621,10 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4">
         <v>11</v>
@@ -685,10 +686,10 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8">
         <v>15</v>
@@ -697,10 +698,10 @@
         <v>16</v>
       </c>
       <c r="K8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" t="s">
         <v>30</v>
-      </c>
-      <c r="L8" t="s">
-        <v>31</v>
       </c>
       <c r="M8">
         <v>14</v>
@@ -729,10 +730,10 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9">
         <v>16</v>
@@ -741,10 +742,10 @@
         <v>17</v>
       </c>
       <c r="K9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" t="s">
         <v>30</v>
-      </c>
-      <c r="L9" t="s">
-        <v>31</v>
       </c>
       <c r="M9">
         <v>14</v>
@@ -773,10 +774,10 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10">
         <v>17</v>
@@ -805,10 +806,10 @@
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I11">
         <v>18</v>
@@ -837,10 +838,10 @@
         <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I12">
         <v>19</v>
@@ -869,10 +870,10 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I13">
         <v>20</v>
@@ -881,10 +882,10 @@
         <v>21</v>
       </c>
       <c r="K13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" t="s">
         <v>32</v>
-      </c>
-      <c r="L13" t="s">
-        <v>33</v>
       </c>
       <c r="M13">
         <v>15</v>
@@ -924,10 +925,10 @@
         <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15">
         <v>22</v>
@@ -956,10 +957,10 @@
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I16">
         <v>23</v>
@@ -999,10 +1000,10 @@
         <v>21</v>
       </c>
       <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" t="s">
         <v>28</v>
-      </c>
-      <c r="H18" t="s">
-        <v>29</v>
       </c>
       <c r="I18">
         <v>24</v>
@@ -1011,10 +1012,10 @@
         <v>25</v>
       </c>
       <c r="K18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" t="s">
         <v>34</v>
-      </c>
-      <c r="L18" t="s">
-        <v>35</v>
       </c>
       <c r="M18">
         <v>18</v>
@@ -1043,10 +1044,10 @@
         <v>22</v>
       </c>
       <c r="G19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" t="s">
         <v>36</v>
-      </c>
-      <c r="H19" t="s">
-        <v>37</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1075,10 +1076,10 @@
         <v>21</v>
       </c>
       <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
         <v>28</v>
-      </c>
-      <c r="H20" t="s">
-        <v>29</v>
       </c>
       <c r="I20">
         <v>24</v>
@@ -1087,10 +1088,10 @@
         <v>25</v>
       </c>
       <c r="K20" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" t="s">
         <v>34</v>
-      </c>
-      <c r="L20" t="s">
-        <v>35</v>
       </c>
       <c r="M20">
         <v>18</v>
@@ -1119,10 +1120,10 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
         <v>36</v>
-      </c>
-      <c r="H21" t="s">
-        <v>37</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1151,10 +1152,10 @@
         <v>22</v>
       </c>
       <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
         <v>28</v>
-      </c>
-      <c r="H22" t="s">
-        <v>29</v>
       </c>
       <c r="I22">
         <v>25</v>
@@ -1163,10 +1164,10 @@
         <v>26</v>
       </c>
       <c r="K22" t="s">
+        <v>33</v>
+      </c>
+      <c r="L22" t="s">
         <v>34</v>
-      </c>
-      <c r="L22" t="s">
-        <v>35</v>
       </c>
       <c r="M22">
         <v>18</v>
@@ -1195,10 +1196,10 @@
         <v>22</v>
       </c>
       <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
         <v>36</v>
-      </c>
-      <c r="H23" t="s">
-        <v>37</v>
       </c>
       <c r="I23">
         <v>3</v>
@@ -1227,10 +1228,10 @@
         <v>23</v>
       </c>
       <c r="G24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" t="s">
         <v>28</v>
-      </c>
-      <c r="H24" t="s">
-        <v>29</v>
       </c>
       <c r="I24">
         <v>27</v>
@@ -1239,10 +1240,10 @@
         <v>28</v>
       </c>
       <c r="K24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24" t="s">
         <v>34</v>
-      </c>
-      <c r="L24" t="s">
-        <v>35</v>
       </c>
       <c r="M24">
         <v>18</v>
@@ -1317,7 +1318,27 @@
         <v>7</v>
       </c>
     </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f>COUNT(A2:A30)</f>
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631A88F7-3653-434B-9A87-7F9CDC25F281}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added helper function get_locus_tags
</commit_message>
<xml_diff>
--- a/PracticeSheet.xlsx
+++ b/PracticeSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhkh\Documents\UBC\COOP\S2019 CARDONA LAB\High Density Transposon Mutant Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF1A8F-E658-40EF-B932-5BDD2EA1270B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57E78BA-C211-4884-9F67-F54799048846}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1296" yWindow="1126" windowWidth="18851" windowHeight="10302" xr2:uid="{F2D4EA85-3696-4C72-B544-258F025EF0EE}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="14374" xr2:uid="{F2D4EA85-3696-4C72-B544-258F025EF0EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,16 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t>e</t>
   </si>
@@ -146,6 +137,21 @@
   </si>
   <si>
     <t>Locus TAG</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>lse</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>position</t>
   </si>
 </sst>
 </file>
@@ -497,44 +503,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD4661C-C763-4B6E-9515-401C70A35075}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -557,10 +563,10 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I2">
         <v>9</v>
@@ -589,10 +595,10 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I3">
         <v>10</v>
@@ -609,7 +615,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -621,10 +627,10 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I4">
         <v>11</v>
@@ -641,7 +647,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -652,7 +658,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -663,7 +669,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -686,10 +692,10 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I8">
         <v>15</v>
@@ -698,10 +704,10 @@
         <v>16</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M8">
         <v>14</v>
@@ -730,10 +736,10 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I9">
         <v>16</v>
@@ -742,10 +748,10 @@
         <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M9">
         <v>14</v>
@@ -762,7 +768,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>12</v>
@@ -774,10 +780,10 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I10">
         <v>17</v>
@@ -794,7 +800,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>13</v>
@@ -806,10 +812,10 @@
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I11">
         <v>18</v>
@@ -826,7 +832,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>14</v>
@@ -838,10 +844,10 @@
         <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I12">
         <v>19</v>
@@ -870,10 +876,10 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I13">
         <v>20</v>
@@ -882,10 +888,10 @@
         <v>21</v>
       </c>
       <c r="K13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M13">
         <v>15</v>
@@ -902,7 +908,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -925,10 +931,10 @@
         <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I15">
         <v>22</v>
@@ -957,10 +963,10 @@
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I16">
         <v>23</v>
@@ -969,7 +975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -977,10 +983,10 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1000,10 +1006,10 @@
         <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I18">
         <v>24</v>
@@ -1012,10 +1018,10 @@
         <v>25</v>
       </c>
       <c r="K18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M18">
         <v>18</v>
@@ -1024,7 +1030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>20</v>
@@ -1044,10 +1050,10 @@
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1056,7 +1062,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1076,10 +1082,10 @@
         <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I20">
         <v>24</v>
@@ -1088,10 +1094,10 @@
         <v>25</v>
       </c>
       <c r="K20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M20">
         <v>18</v>
@@ -1099,8 +1105,20 @@
       <c r="N20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>35</v>
+      </c>
+      <c r="P20" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q20">
+        <v>18</v>
+      </c>
+      <c r="R20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1108,7 +1126,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -1120,10 +1138,10 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1132,7 +1150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1152,10 +1170,10 @@
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I22">
         <v>25</v>
@@ -1164,10 +1182,10 @@
         <v>26</v>
       </c>
       <c r="K22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M22">
         <v>18</v>
@@ -1176,7 +1194,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>18</v>
       </c>
@@ -1184,7 +1202,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D23">
         <v>20</v>
@@ -1196,10 +1214,10 @@
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I23">
         <v>3</v>
@@ -1208,7 +1226,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1228,10 +1246,10 @@
         <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I24">
         <v>27</v>
@@ -1240,10 +1258,10 @@
         <v>28</v>
       </c>
       <c r="K24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M24">
         <v>18</v>
@@ -1252,7 +1270,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1260,10 +1278,10 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1271,10 +1289,10 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1282,10 +1300,10 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1293,10 +1311,10 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1304,10 +1322,10 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1315,10 +1333,10 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <f>COUNT(A2:A30)</f>
         <v>29</v>

</xml_diff>